<commit_message>
add api for guru page
</commit_message>
<xml_diff>
--- a/controllers/absensi_bulan_ini.xlsx
+++ b/controllers/absensi_bulan_ini.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Nama Siswa</t>
   </si>
@@ -22,61 +22,25 @@
     <t>Minggu ke-1</t>
   </si>
   <si>
-    <t>Minggu ke-3</t>
-  </si>
-  <si>
-    <t>Minggu ke-4</t>
-  </si>
-  <si>
-    <t>Minggu ke-5</t>
-  </si>
-  <si>
     <t>Total Pertemuan</t>
   </si>
   <si>
     <t>Jumlah Hadir</t>
   </si>
   <si>
-    <t>Angelita Natali</t>
-  </si>
-  <si>
-    <t>7</t>
+    <t>Bram Felix Sitinjak</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>Hadir</t>
   </si>
   <si>
-    <t>Evelyn Supratna</t>
+    <t>Cheeryl Paulina Ginto</t>
   </si>
   <si>
     <t>Absen</t>
-  </si>
-  <si>
-    <t>Felix Hizkia Lorentius</t>
-  </si>
-  <si>
-    <t>Axel Alvaro</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Bram Felix Sitinjak</t>
-  </si>
-  <si>
-    <t>Caesar Alexander</t>
-  </si>
-  <si>
-    <t>Daniel Enrico Siswanto</t>
-  </si>
-  <si>
-    <t>Gabriella Lintang S. Kingkin</t>
-  </si>
-  <si>
-    <t>Gregorius Fabian Lentiny Rehing</t>
-  </si>
-  <si>
-    <t>Kai Jasiello Bofyana</t>
   </si>
 </sst>
 </file>
@@ -469,15 +433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:E3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="8" width="15" customWidth="1"/>
+    <col min="3" max="5" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,274 +457,39 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
+      <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10">
-        <v>4</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>4</v>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>